<commit_message>
support unwanted space field
</commit_message>
<xml_diff>
--- a/iLease/Example.xlsx
+++ b/iLease/Example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Confic" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>A0001</t>
   </si>
@@ -206,13 +206,22 @@
   </si>
   <si>
     <t>Sheet1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ส่วนแบ่งhubCollection</t>
+  </si>
+  <si>
+    <t>เพิ่มเปอร์เซ็นต์hubcollection_button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,6 +242,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="9">
@@ -366,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -397,6 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1154,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1268,6 +1285,11 @@
         <v>44</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1275,18 +1297,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="6.5" style="25" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="18" max="18" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>24</v>
       </c>
@@ -1313,12 +1337,37 @@
         <v>3</v>
       </c>
       <c r="J1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-    </row>
-    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="24"/>
       <c r="C2" s="22" t="s">
@@ -1337,16 +1386,39 @@
         <v>54</v>
       </c>
       <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="14" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14">
+        <v>5</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>50</v>
       </c>
@@ -1359,6 +1431,9 @@
       </c>
       <c r="H3" t="s">
         <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>